<commit_message>
Add cpp code for questions 3-5
</commit_message>
<xml_diff>
--- a/Love Babbar 450 DSA Questions/FINAL450.xlsx
+++ b/Love Babbar 450 DSA Questions/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\450-dsa-questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\dsa\Love Babbar 450 DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFDF0A4-10D3-4707-A642-E22F7067CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF87DD9-1678-4E5A-A9EC-E16D0A39C764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="487">
   <si>
     <t>Topic:</t>
   </si>
@@ -1483,6 +1483,15 @@
   </si>
   <si>
     <t>MinAndMax.cpp</t>
+  </si>
+  <si>
+    <t>KthSmallestElement.cpp</t>
+  </si>
+  <si>
+    <t>Sort0s1s2s.cpp</t>
+  </si>
+  <si>
+    <t>MoveNegativeToStartPositiveToEnd.cpp</t>
   </si>
 </sst>
 </file>
@@ -1925,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2008,6 +2017,9 @@
       <c r="D5" s="8" t="s">
         <v>466</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -2022,6 +2034,9 @@
       <c r="D6" s="8" t="s">
         <v>469</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -2035,6 +2050,9 @@
       </c>
       <c r="D7" s="8" t="s">
         <v>470</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add cpp code for questions 6-13
</commit_message>
<xml_diff>
--- a/Love Babbar 450 DSA Questions/FINAL450.xlsx
+++ b/Love Babbar 450 DSA Questions/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\dsa\Love Babbar 450 DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF87DD9-1678-4E5A-A9EC-E16D0A39C764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5780D5-7880-4828-BA4A-C578CA3DEEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="494">
   <si>
     <t>Topic:</t>
   </si>
@@ -1492,6 +1492,27 @@
   </si>
   <si>
     <t>MoveNegativeToStartPositiveToEnd.cpp</t>
+  </si>
+  <si>
+    <t>UnionAndIntersection.cpp</t>
+  </si>
+  <si>
+    <t>RotateBy1.cpp</t>
+  </si>
+  <si>
+    <t>LargestSumContiguousSubarray.cpp</t>
+  </si>
+  <si>
+    <t>MinimizeTheHeights.cpp</t>
+  </si>
+  <si>
+    <t>MinNumOfJumpsToReachEnd.cpp</t>
+  </si>
+  <si>
+    <t>FindDuplicate.cpp</t>
+  </si>
+  <si>
+    <t>MergeSortedWithoutExtraSpace.cpp</t>
   </si>
 </sst>
 </file>
@@ -1934,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1943,8 +1964,8 @@
     <col min="1" max="1" width="25.875" customWidth="1"/>
     <col min="2" max="2" width="113.125" customWidth="1"/>
     <col min="3" max="3" width="13.625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="39.375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="40.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="40.25" style="8" customWidth="1"/>
+    <col min="5" max="5" width="39.375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1958,10 +1979,10 @@
         <v>462</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1981,10 +2002,10 @@
         <v>463</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>465</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -1998,10 +2019,10 @@
         <v>463</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>467</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2015,10 +2036,10 @@
         <v>463</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>466</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2032,10 +2053,10 @@
         <v>463</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>469</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2049,10 +2070,10 @@
         <v>463</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>470</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2066,6 +2087,9 @@
         <v>463</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>471</v>
       </c>
     </row>
@@ -2080,6 +2104,9 @@
         <v>463</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>472</v>
       </c>
     </row>
@@ -2094,6 +2121,9 @@
         <v>463</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>473</v>
       </c>
     </row>
@@ -2108,6 +2138,9 @@
         <v>463</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>474</v>
       </c>
     </row>
@@ -2122,6 +2155,9 @@
         <v>463</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>475</v>
       </c>
     </row>
@@ -2136,6 +2172,9 @@
         <v>463</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>476</v>
       </c>
     </row>
@@ -2150,6 +2189,9 @@
         <v>463</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>477</v>
       </c>
     </row>
@@ -2164,6 +2206,9 @@
         <v>463</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>473</v>
       </c>
     </row>
@@ -2177,11 +2222,11 @@
       <c r="C16" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -2191,11 +2236,11 @@
       <c r="C17" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>3</v>
       </c>
@@ -2205,11 +2250,11 @@
       <c r="C18" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2220,7 +2265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -2231,7 +2276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2242,7 +2287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
@@ -2253,7 +2298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -2275,7 +2320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -2286,7 +2331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -2297,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -2308,7 +2353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -2319,7 +2364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -2330,7 +2375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -2341,7 +2386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -2352,7 +2397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Add cpp code for questions 14-18
</commit_message>
<xml_diff>
--- a/Love Babbar 450 DSA Questions/FINAL450.xlsx
+++ b/Love Babbar 450 DSA Questions/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\dsa\Love Babbar 450 DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5780D5-7880-4828-BA4A-C578CA3DEEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAAEEC8-FDB8-4FD5-A623-C27973BA95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="499">
   <si>
     <t>Topic:</t>
   </si>
@@ -1513,6 +1513,21 @@
   </si>
   <si>
     <t>MergeSortedWithoutExtraSpace.cpp</t>
+  </si>
+  <si>
+    <t>MergeIntervals.cpp</t>
+  </si>
+  <si>
+    <t>NextPermutation.cpp</t>
+  </si>
+  <si>
+    <t>CountInversions.cpp</t>
+  </si>
+  <si>
+    <t>MaximizeProfit.cpp</t>
+  </si>
+  <si>
+    <t>CountPairsWithSameSum.cpp</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1971,7 @@
   <dimension ref="A1:E478"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2222,6 +2237,9 @@
       <c r="C16" s="9" t="s">
         <v>463</v>
       </c>
+      <c r="D16" s="8" t="s">
+        <v>494</v>
+      </c>
       <c r="E16" s="8" t="s">
         <v>478</v>
       </c>
@@ -2236,6 +2254,9 @@
       <c r="C17" s="9" t="s">
         <v>463</v>
       </c>
+      <c r="D17" s="8" t="s">
+        <v>495</v>
+      </c>
       <c r="E17" s="8" t="s">
         <v>479</v>
       </c>
@@ -2250,6 +2271,9 @@
       <c r="C18" s="9" t="s">
         <v>463</v>
       </c>
+      <c r="D18" s="8" t="s">
+        <v>496</v>
+      </c>
       <c r="E18" s="8" t="s">
         <v>480</v>
       </c>
@@ -2262,7 +2286,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2273,7 +2300,10 @@
         <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add cpp code for questions 19-30
</commit_message>
<xml_diff>
--- a/Love Babbar 450 DSA Questions/FINAL450.xlsx
+++ b/Love Babbar 450 DSA Questions/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\dsa\Love Babbar 450 DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAAEEC8-FDB8-4FD5-A623-C27973BA95E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A48CF2C-20BF-4CC6-986D-316E6351FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="511">
   <si>
     <t>Topic:</t>
   </si>
@@ -1528,6 +1528,42 @@
   </si>
   <si>
     <t>CountPairsWithSameSum.cpp</t>
+  </si>
+  <si>
+    <t>CommonElements.cpp</t>
+  </si>
+  <si>
+    <t>AlternatePositiveNegative.cpp</t>
+  </si>
+  <si>
+    <t>SubarrayWith0Sum.cpp</t>
+  </si>
+  <si>
+    <t>FactorialOfLargeNumbers.cpp</t>
+  </si>
+  <si>
+    <t>MaximumProductSubarray.cpp</t>
+  </si>
+  <si>
+    <t>LongestConsecutiveSubsequence.cpp</t>
+  </si>
+  <si>
+    <t>FindElementsAppearingMoreThanNbyK.cpp</t>
+  </si>
+  <si>
+    <t>MaxProfitBuyingSellingAtmostTwice.cpp</t>
+  </si>
+  <si>
+    <t>CheckIfArrayIsSubsetOfAnother.cpp</t>
+  </si>
+  <si>
+    <t>TripletSum.cpp</t>
+  </si>
+  <si>
+    <t>TrappingRainwater.cpp</t>
+  </si>
+  <si>
+    <t>ChocolateDistribution.cpp</t>
   </si>
 </sst>
 </file>
@@ -1970,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2314,7 +2350,10 @@
         <v>22</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2325,29 +2364,38 @@
         <v>23</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2358,18 +2406,24 @@
         <v>26</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2380,18 +2434,24 @@
         <v>28</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2402,7 +2462,10 @@
         <v>30</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2413,18 +2476,24 @@
         <v>31</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -2435,7 +2504,10 @@
         <v>33</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>2</v>
+        <v>463</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -7171,424 +7243,424 @@
     <hyperlink ref="B28" r:id="rId25" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
     <hyperlink ref="B29" r:id="rId26" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
     <hyperlink ref="B30" r:id="rId27" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
-    <hyperlink ref="B31" r:id="rId28" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
-    <hyperlink ref="B32" r:id="rId29" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
-    <hyperlink ref="B33" r:id="rId30" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
-    <hyperlink ref="B34" r:id="rId31" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
-    <hyperlink ref="B35" r:id="rId32" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="B36" r:id="rId33" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="B37" r:id="rId34" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="B38" r:id="rId35" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
-    <hyperlink ref="B41" r:id="rId36" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
-    <hyperlink ref="B42" r:id="rId37" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="B43" r:id="rId38" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="B44" r:id="rId39" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="B45" r:id="rId40" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="B46" r:id="rId41" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="B47" r:id="rId42" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="B48" r:id="rId43" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="B49" r:id="rId44" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="B50" r:id="rId45" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="B53" r:id="rId46" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="B54" r:id="rId47" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
-    <hyperlink ref="B55" r:id="rId48" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
-    <hyperlink ref="B57" r:id="rId49" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
-    <hyperlink ref="B58" r:id="rId50" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
-    <hyperlink ref="B59" r:id="rId51" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
-    <hyperlink ref="B60" r:id="rId52" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
-    <hyperlink ref="B61" r:id="rId53" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
-    <hyperlink ref="B62" r:id="rId54" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
-    <hyperlink ref="B63" r:id="rId55" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
-    <hyperlink ref="B64" r:id="rId56" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
-    <hyperlink ref="B65" r:id="rId57" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
-    <hyperlink ref="B66" r:id="rId58" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
-    <hyperlink ref="B67" r:id="rId59" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
-    <hyperlink ref="B68" r:id="rId60" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
-    <hyperlink ref="B69" r:id="rId61" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
-    <hyperlink ref="B70" r:id="rId62" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
-    <hyperlink ref="B71" r:id="rId63" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
-    <hyperlink ref="B72" r:id="rId64" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
-    <hyperlink ref="B73" r:id="rId65" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
-    <hyperlink ref="B74" r:id="rId66" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
-    <hyperlink ref="B75" r:id="rId67" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
-    <hyperlink ref="B76" r:id="rId68" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
-    <hyperlink ref="B77" r:id="rId69" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
-    <hyperlink ref="B78" r:id="rId70" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
-    <hyperlink ref="B79" r:id="rId71" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
-    <hyperlink ref="B80" r:id="rId72" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
-    <hyperlink ref="B81" r:id="rId73" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
-    <hyperlink ref="B82" r:id="rId74" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
-    <hyperlink ref="B83" r:id="rId75" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="B84" r:id="rId76" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="B85" r:id="rId77" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="B86" r:id="rId78" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="B87" r:id="rId79" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="B88" r:id="rId80" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="B89" r:id="rId81" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="B90" r:id="rId82" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="B91" r:id="rId83" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="B92" r:id="rId84" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="B93" r:id="rId85" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="B94" r:id="rId86" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="B95" r:id="rId87" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="B98" r:id="rId88" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="B99" r:id="rId89" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="B100" r:id="rId90" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="B101" r:id="rId91" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="B103" r:id="rId92" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="B104" r:id="rId93" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="B105" r:id="rId94" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="B106" r:id="rId95" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="B107" r:id="rId96" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="B108" r:id="rId97" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="B110" r:id="rId98" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="B111" r:id="rId99" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="B112" r:id="rId100" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="B113" r:id="rId101" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="B114" r:id="rId102" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="B115" r:id="rId103" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="B116" r:id="rId104" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="B117" r:id="rId105" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="B118" r:id="rId106" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="B119" r:id="rId107" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="B120" r:id="rId108" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="B121" r:id="rId109" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="B122" r:id="rId110" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="B123" r:id="rId111" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="B124" r:id="rId112" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="B125" r:id="rId113" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="B126" r:id="rId114" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="B127" r:id="rId115" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="B128" r:id="rId116" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="B129" r:id="rId117" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="B130" r:id="rId118" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="B131" r:id="rId119" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="B132" r:id="rId120" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="B133" r:id="rId121" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="B102" r:id="rId122" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="B109" r:id="rId123" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="B136" r:id="rId124" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="B137" r:id="rId125" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="B138" r:id="rId126" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="B139" r:id="rId127" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="B140" r:id="rId128" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="B141" r:id="rId129" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="B142" r:id="rId130" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="B143" r:id="rId131" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="B144" r:id="rId132" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="B145" r:id="rId133" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="B146" r:id="rId134" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="B147" r:id="rId135" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="B148" r:id="rId136" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="B149" r:id="rId137" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="B150" r:id="rId138" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="B151" r:id="rId139" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="B152" r:id="rId140" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="B153" r:id="rId141" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="B154" r:id="rId142" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="B155" r:id="rId143" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="B156" r:id="rId144" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="B157" r:id="rId145" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="B158" r:id="rId146" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="B159" r:id="rId147" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="B160" r:id="rId148" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="B163" r:id="rId149" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="B164" r:id="rId150" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="B165" r:id="rId151" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="B166" r:id="rId152" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="B167" r:id="rId153" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="B168" r:id="rId154" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="B169" r:id="rId155" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="B170" r:id="rId156" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="B171" r:id="rId157" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B174" r:id="rId158" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B175" r:id="rId159" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B176" r:id="rId160" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B177" r:id="rId161" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B178" r:id="rId162" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B179" r:id="rId163" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B180" r:id="rId164" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B181" r:id="rId165" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B182" r:id="rId166" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B183" r:id="rId167" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B184" r:id="rId168" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B185" r:id="rId169" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B186" r:id="rId170" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B187" r:id="rId171" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B188" r:id="rId172" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B189" r:id="rId173" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B190" r:id="rId174" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B191" r:id="rId175" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B192" r:id="rId176" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B193" r:id="rId177" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B194" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B195" r:id="rId179" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B196" r:id="rId180" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B197" r:id="rId181" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B198" r:id="rId182" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B199" r:id="rId183" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B200" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B201" r:id="rId185" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B202" r:id="rId186" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B203" r:id="rId187" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B204" r:id="rId188" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B205" r:id="rId189" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B206" r:id="rId190" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B207" r:id="rId191" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B208" r:id="rId192" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B211" r:id="rId193" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B212" r:id="rId194" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B213" r:id="rId195" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B214" r:id="rId196" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B215" r:id="rId197" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B216" r:id="rId198" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B217" r:id="rId199" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B218" r:id="rId200" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B219" r:id="rId201" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B220" r:id="rId202" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B221" r:id="rId203" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B222" r:id="rId204" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B223" r:id="rId205" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B224" r:id="rId206" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B225" r:id="rId207" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B226" r:id="rId208" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B227" r:id="rId209" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B228" r:id="rId210" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B229" r:id="rId211" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B230" r:id="rId212" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B231" r:id="rId213" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B232" r:id="rId214" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B235" r:id="rId215" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B236" r:id="rId216" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B237" r:id="rId217" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B238" r:id="rId218" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B239" r:id="rId219" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B240" r:id="rId220" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B241" r:id="rId221" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B242" r:id="rId222" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B243" r:id="rId223" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B244" r:id="rId224" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B245" r:id="rId225" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B246" r:id="rId226" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B247" r:id="rId227" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B248" r:id="rId228" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B249" r:id="rId229" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B250" r:id="rId230" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B251" r:id="rId231" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B252" r:id="rId232" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B253" r:id="rId233" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B254" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B255" r:id="rId235" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B256" r:id="rId236" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B257" r:id="rId237" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B258" r:id="rId238" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B259" r:id="rId239" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B260" r:id="rId240" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B261" r:id="rId241" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B262" r:id="rId242" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B263" r:id="rId243" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B264" r:id="rId244" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B265" r:id="rId245" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B266" r:id="rId246" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B267" r:id="rId247" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B268" r:id="rId248" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B269" r:id="rId249" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B272" r:id="rId250" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B273" r:id="rId251" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B274" r:id="rId252" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B275" r:id="rId253" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B276" r:id="rId254" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B277" r:id="rId255" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B278" r:id="rId256" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B279" r:id="rId257" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B280" r:id="rId258" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B281" r:id="rId259" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B282" r:id="rId260" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B283" r:id="rId261" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B284" r:id="rId262" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B285" r:id="rId263" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B286" r:id="rId264" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B287" r:id="rId265" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B288" r:id="rId266" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B289" r:id="rId267" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B290" r:id="rId268" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B293" r:id="rId269" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B294" r:id="rId270" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B295" r:id="rId271" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B296" r:id="rId272" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B297" r:id="rId273" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B298" r:id="rId274" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B299" r:id="rId275" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B300" r:id="rId276" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B301" r:id="rId277" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B302" r:id="rId278" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B303" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B304" r:id="rId280" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B305" r:id="rId281" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B306" r:id="rId282" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B307" r:id="rId283" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B308" r:id="rId284" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B309" r:id="rId285" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B310" r:id="rId286" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B311" r:id="rId287" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B312" r:id="rId288" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B313" r:id="rId289" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B314" r:id="rId290" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B315" r:id="rId291" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B316" r:id="rId292" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B317" r:id="rId293" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B318" r:id="rId294" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B319" r:id="rId295" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B320" r:id="rId296" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B321" r:id="rId297" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B322" r:id="rId298" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B323" r:id="rId299" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B324" r:id="rId300" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B325" r:id="rId301" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B326" r:id="rId302" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B327" r:id="rId303" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B328" r:id="rId304" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B329" r:id="rId305" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B330" r:id="rId306" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B333" r:id="rId307" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B334" r:id="rId308" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B335" r:id="rId309" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B336" r:id="rId310" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B337" r:id="rId311" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B338" r:id="rId312" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B339" r:id="rId313" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B340" r:id="rId314" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B341" r:id="rId315" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B342" r:id="rId316" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B343" r:id="rId317" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B344" r:id="rId318" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B345" r:id="rId319" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B346" r:id="rId320" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B347" r:id="rId321" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B348" r:id="rId322" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B349" r:id="rId323" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B350" r:id="rId324" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B354" r:id="rId325" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B355" r:id="rId326" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B356" r:id="rId327" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B357" r:id="rId328" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B358" r:id="rId329" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B359" r:id="rId330" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B360" r:id="rId331" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B361" r:id="rId332" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B362" r:id="rId333" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B363" r:id="rId334" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B364" r:id="rId335" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B365" r:id="rId336" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B366" r:id="rId337" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B367" r:id="rId338" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B368" r:id="rId339" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B369" r:id="rId340" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B370" r:id="rId341" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B371" r:id="rId342" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B372" r:id="rId343" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B373" r:id="rId344" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B374" r:id="rId345" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B375" r:id="rId346" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B376" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B377" r:id="rId348" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B378" r:id="rId349" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B379" r:id="rId350" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B380" r:id="rId351" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B381" r:id="rId352" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B382" r:id="rId353" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B383" r:id="rId354" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B384" r:id="rId355" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B385" r:id="rId356" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B386" r:id="rId357" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B387" r:id="rId358" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B388" r:id="rId359" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B389" r:id="rId360" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B390" r:id="rId361" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B391" r:id="rId362" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B393" r:id="rId363" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B392" r:id="rId364" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B394" r:id="rId365" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B395" r:id="rId366" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B396" r:id="rId367" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B399" r:id="rId368" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B400" r:id="rId369" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B401" r:id="rId370" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B402" r:id="rId371" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B403" r:id="rId372" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B404" r:id="rId373" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B407" r:id="rId374" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B408" r:id="rId375" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B409" r:id="rId376" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B410" r:id="rId377" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B411" r:id="rId378" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B412" r:id="rId379" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B413" r:id="rId380" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B414" r:id="rId381" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B415" r:id="rId382" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B416" r:id="rId383" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B417" r:id="rId384" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B418" r:id="rId385" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B419" r:id="rId386" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B420" r:id="rId387" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B421" r:id="rId388" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B422" r:id="rId389" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B423" r:id="rId390" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B424" r:id="rId391" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B425" r:id="rId392" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B426" r:id="rId393" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B427" r:id="rId394" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B428" r:id="rId395" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B429" r:id="rId396" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B430" r:id="rId397" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B431" r:id="rId398" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B432" r:id="rId399" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B433" r:id="rId400" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B434" r:id="rId401" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B435" r:id="rId402" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B436" r:id="rId403" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B437" r:id="rId404" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B438" r:id="rId405" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B439" r:id="rId406" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B440" r:id="rId407" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B441" r:id="rId408" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B442" r:id="rId409" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B443" r:id="rId410" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B444" r:id="rId411" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B445" r:id="rId412" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B446" r:id="rId413" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B448" r:id="rId414" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B447" r:id="rId415" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B449" r:id="rId416" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B450" r:id="rId417" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B451" r:id="rId418" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B452" r:id="rId419" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B453" r:id="rId420" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B454" r:id="rId421" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B455" r:id="rId422" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B456" r:id="rId423" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B457" r:id="rId424" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B458" r:id="rId425" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B459" r:id="rId426" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B466" r:id="rId427" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B465" r:id="rId428" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B464" r:id="rId429" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B463" r:id="rId430" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B462" r:id="rId431" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B461" r:id="rId432" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B460" r:id="rId433" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B469" r:id="rId434" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B470" r:id="rId435" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B471" r:id="rId436" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B472" r:id="rId437" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B473" r:id="rId438" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B474" r:id="rId439" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B475" r:id="rId440" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B478" r:id="rId441" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B476" r:id="rId442" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B477" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B353" r:id="rId444" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="B12" r:id="rId445" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
+    <hyperlink ref="B32" r:id="rId28" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
+    <hyperlink ref="B33" r:id="rId29" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
+    <hyperlink ref="B34" r:id="rId30" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
+    <hyperlink ref="B35" r:id="rId31" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
+    <hyperlink ref="B36" r:id="rId32" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
+    <hyperlink ref="B38" r:id="rId34" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
+    <hyperlink ref="B41" r:id="rId35" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="B42" r:id="rId36" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
+    <hyperlink ref="B43" r:id="rId37" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
+    <hyperlink ref="B44" r:id="rId38" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
+    <hyperlink ref="B45" r:id="rId39" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
+    <hyperlink ref="B46" r:id="rId40" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
+    <hyperlink ref="B47" r:id="rId41" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
+    <hyperlink ref="B48" r:id="rId42" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
+    <hyperlink ref="B49" r:id="rId43" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
+    <hyperlink ref="B50" r:id="rId44" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
+    <hyperlink ref="B53" r:id="rId45" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
+    <hyperlink ref="B54" r:id="rId46" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
+    <hyperlink ref="B55" r:id="rId47" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
+    <hyperlink ref="B57" r:id="rId48" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
+    <hyperlink ref="B58" r:id="rId49" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
+    <hyperlink ref="B59" r:id="rId50" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
+    <hyperlink ref="B60" r:id="rId51" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
+    <hyperlink ref="B61" r:id="rId52" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
+    <hyperlink ref="B62" r:id="rId53" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
+    <hyperlink ref="B63" r:id="rId54" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
+    <hyperlink ref="B64" r:id="rId55" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
+    <hyperlink ref="B65" r:id="rId56" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
+    <hyperlink ref="B66" r:id="rId57" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
+    <hyperlink ref="B67" r:id="rId58" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
+    <hyperlink ref="B68" r:id="rId59" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
+    <hyperlink ref="B69" r:id="rId60" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
+    <hyperlink ref="B70" r:id="rId61" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
+    <hyperlink ref="B71" r:id="rId62" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
+    <hyperlink ref="B72" r:id="rId63" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
+    <hyperlink ref="B73" r:id="rId64" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
+    <hyperlink ref="B74" r:id="rId65" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
+    <hyperlink ref="B75" r:id="rId66" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
+    <hyperlink ref="B76" r:id="rId67" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
+    <hyperlink ref="B77" r:id="rId68" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
+    <hyperlink ref="B78" r:id="rId69" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
+    <hyperlink ref="B79" r:id="rId70" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
+    <hyperlink ref="B80" r:id="rId71" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
+    <hyperlink ref="B81" r:id="rId72" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
+    <hyperlink ref="B82" r:id="rId73" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
+    <hyperlink ref="B83" r:id="rId74" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
+    <hyperlink ref="B84" r:id="rId75" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
+    <hyperlink ref="B85" r:id="rId76" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="B86" r:id="rId77" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="B87" r:id="rId78" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="B88" r:id="rId79" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="B89" r:id="rId80" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="B90" r:id="rId81" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="B91" r:id="rId82" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="B92" r:id="rId83" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="B93" r:id="rId84" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="B94" r:id="rId85" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="B95" r:id="rId86" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="B98" r:id="rId87" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
+    <hyperlink ref="B99" r:id="rId88" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
+    <hyperlink ref="B100" r:id="rId89" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
+    <hyperlink ref="B101" r:id="rId90" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
+    <hyperlink ref="B103" r:id="rId91" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
+    <hyperlink ref="B104" r:id="rId92" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
+    <hyperlink ref="B105" r:id="rId93" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
+    <hyperlink ref="B106" r:id="rId94" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
+    <hyperlink ref="B107" r:id="rId95" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
+    <hyperlink ref="B108" r:id="rId96" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
+    <hyperlink ref="B110" r:id="rId97" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
+    <hyperlink ref="B111" r:id="rId98" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
+    <hyperlink ref="B112" r:id="rId99" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
+    <hyperlink ref="B113" r:id="rId100" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
+    <hyperlink ref="B114" r:id="rId101" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
+    <hyperlink ref="B115" r:id="rId102" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="B116" r:id="rId103" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
+    <hyperlink ref="B117" r:id="rId104" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
+    <hyperlink ref="B118" r:id="rId105" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
+    <hyperlink ref="B119" r:id="rId106" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
+    <hyperlink ref="B120" r:id="rId107" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
+    <hyperlink ref="B121" r:id="rId108" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
+    <hyperlink ref="B122" r:id="rId109" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
+    <hyperlink ref="B123" r:id="rId110" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
+    <hyperlink ref="B124" r:id="rId111" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
+    <hyperlink ref="B125" r:id="rId112" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
+    <hyperlink ref="B126" r:id="rId113" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
+    <hyperlink ref="B127" r:id="rId114" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
+    <hyperlink ref="B128" r:id="rId115" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
+    <hyperlink ref="B129" r:id="rId116" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
+    <hyperlink ref="B130" r:id="rId117" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
+    <hyperlink ref="B131" r:id="rId118" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
+    <hyperlink ref="B132" r:id="rId119" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
+    <hyperlink ref="B133" r:id="rId120" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
+    <hyperlink ref="B102" r:id="rId121" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
+    <hyperlink ref="B109" r:id="rId122" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
+    <hyperlink ref="B136" r:id="rId123" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
+    <hyperlink ref="B137" r:id="rId124" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
+    <hyperlink ref="B138" r:id="rId125" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
+    <hyperlink ref="B139" r:id="rId126" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
+    <hyperlink ref="B140" r:id="rId127" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
+    <hyperlink ref="B141" r:id="rId128" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
+    <hyperlink ref="B142" r:id="rId129" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
+    <hyperlink ref="B143" r:id="rId130" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
+    <hyperlink ref="B144" r:id="rId131" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
+    <hyperlink ref="B145" r:id="rId132" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
+    <hyperlink ref="B146" r:id="rId133" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
+    <hyperlink ref="B147" r:id="rId134" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
+    <hyperlink ref="B148" r:id="rId135" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
+    <hyperlink ref="B149" r:id="rId136" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
+    <hyperlink ref="B150" r:id="rId137" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
+    <hyperlink ref="B151" r:id="rId138" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
+    <hyperlink ref="B152" r:id="rId139" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
+    <hyperlink ref="B153" r:id="rId140" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
+    <hyperlink ref="B154" r:id="rId141" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
+    <hyperlink ref="B155" r:id="rId142" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
+    <hyperlink ref="B156" r:id="rId143" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
+    <hyperlink ref="B157" r:id="rId144" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
+    <hyperlink ref="B158" r:id="rId145" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
+    <hyperlink ref="B159" r:id="rId146" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
+    <hyperlink ref="B160" r:id="rId147" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
+    <hyperlink ref="B163" r:id="rId148" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
+    <hyperlink ref="B164" r:id="rId149" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
+    <hyperlink ref="B165" r:id="rId150" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="B166" r:id="rId151" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="B167" r:id="rId152" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
+    <hyperlink ref="B168" r:id="rId153" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
+    <hyperlink ref="B169" r:id="rId154" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
+    <hyperlink ref="B170" r:id="rId155" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
+    <hyperlink ref="B171" r:id="rId156" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
+    <hyperlink ref="B174" r:id="rId157" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B175" r:id="rId158" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B176" r:id="rId159" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B177" r:id="rId160" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B178" r:id="rId161" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B179" r:id="rId162" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B180" r:id="rId163" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B181" r:id="rId164" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B182" r:id="rId165" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B183" r:id="rId166" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B184" r:id="rId167" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B185" r:id="rId168" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B186" r:id="rId169" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B187" r:id="rId170" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B188" r:id="rId171" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B189" r:id="rId172" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B190" r:id="rId173" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B191" r:id="rId174" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B192" r:id="rId175" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B193" r:id="rId176" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B194" r:id="rId177" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B195" r:id="rId178" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B196" r:id="rId179" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B197" r:id="rId180" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B198" r:id="rId181" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B199" r:id="rId182" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B200" r:id="rId183" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B201" r:id="rId184" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B202" r:id="rId185" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B203" r:id="rId186" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B204" r:id="rId187" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B205" r:id="rId188" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B206" r:id="rId189" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B207" r:id="rId190" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B208" r:id="rId191" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B211" r:id="rId192" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B212" r:id="rId193" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B213" r:id="rId194" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B214" r:id="rId195" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B215" r:id="rId196" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B216" r:id="rId197" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B217" r:id="rId198" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B218" r:id="rId199" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B219" r:id="rId200" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B220" r:id="rId201" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B221" r:id="rId202" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B222" r:id="rId203" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B223" r:id="rId204" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B224" r:id="rId205" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B225" r:id="rId206" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B226" r:id="rId207" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B227" r:id="rId208" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B228" r:id="rId209" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B229" r:id="rId210" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B230" r:id="rId211" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B231" r:id="rId212" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B232" r:id="rId213" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B235" r:id="rId214" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B236" r:id="rId215" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B237" r:id="rId216" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B238" r:id="rId217" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B239" r:id="rId218" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B240" r:id="rId219" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B241" r:id="rId220" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B242" r:id="rId221" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B243" r:id="rId222" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B244" r:id="rId223" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B245" r:id="rId224" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B246" r:id="rId225" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B247" r:id="rId226" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B248" r:id="rId227" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B249" r:id="rId228" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B250" r:id="rId229" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B251" r:id="rId230" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B252" r:id="rId231" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B253" r:id="rId232" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B254" r:id="rId233" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B255" r:id="rId234" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B256" r:id="rId235" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B257" r:id="rId236" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B258" r:id="rId237" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B259" r:id="rId238" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B260" r:id="rId239" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B261" r:id="rId240" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B262" r:id="rId241" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B263" r:id="rId242" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B264" r:id="rId243" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B265" r:id="rId244" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B266" r:id="rId245" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B267" r:id="rId246" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B268" r:id="rId247" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B269" r:id="rId248" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B272" r:id="rId249" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B273" r:id="rId250" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B274" r:id="rId251" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B275" r:id="rId252" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B276" r:id="rId253" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B277" r:id="rId254" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B278" r:id="rId255" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B279" r:id="rId256" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B280" r:id="rId257" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B281" r:id="rId258" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B282" r:id="rId259" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B283" r:id="rId260" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B284" r:id="rId261" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B285" r:id="rId262" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B286" r:id="rId263" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B287" r:id="rId264" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B288" r:id="rId265" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B289" r:id="rId266" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B290" r:id="rId267" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B293" r:id="rId268" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B294" r:id="rId269" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B295" r:id="rId270" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B296" r:id="rId271" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B297" r:id="rId272" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B298" r:id="rId273" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B299" r:id="rId274" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B300" r:id="rId275" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B301" r:id="rId276" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B302" r:id="rId277" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B303" r:id="rId278" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B304" r:id="rId279" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B305" r:id="rId280" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B306" r:id="rId281" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B307" r:id="rId282" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B308" r:id="rId283" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B309" r:id="rId284" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B310" r:id="rId285" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B311" r:id="rId286" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B312" r:id="rId287" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B313" r:id="rId288" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B314" r:id="rId289" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B315" r:id="rId290" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B316" r:id="rId291" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B317" r:id="rId292" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B318" r:id="rId293" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B319" r:id="rId294" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B320" r:id="rId295" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B321" r:id="rId296" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B322" r:id="rId297" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B323" r:id="rId298" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B324" r:id="rId299" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B325" r:id="rId300" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B326" r:id="rId301" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B327" r:id="rId302" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B328" r:id="rId303" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B329" r:id="rId304" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B330" r:id="rId305" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B333" r:id="rId306" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B334" r:id="rId307" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B335" r:id="rId308" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B336" r:id="rId309" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B337" r:id="rId310" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B338" r:id="rId311" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B339" r:id="rId312" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B340" r:id="rId313" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B341" r:id="rId314" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B342" r:id="rId315" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B343" r:id="rId316" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B344" r:id="rId317" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B345" r:id="rId318" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B346" r:id="rId319" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B347" r:id="rId320" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B348" r:id="rId321" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B349" r:id="rId322" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B350" r:id="rId323" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B354" r:id="rId324" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B355" r:id="rId325" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B356" r:id="rId326" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B357" r:id="rId327" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B358" r:id="rId328" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B359" r:id="rId329" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B360" r:id="rId330" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B361" r:id="rId331" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B362" r:id="rId332" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B363" r:id="rId333" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B364" r:id="rId334" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B365" r:id="rId335" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B366" r:id="rId336" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B367" r:id="rId337" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B368" r:id="rId338" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B369" r:id="rId339" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B370" r:id="rId340" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B371" r:id="rId341" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B372" r:id="rId342" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B373" r:id="rId343" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B374" r:id="rId344" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B375" r:id="rId345" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B376" r:id="rId346" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B377" r:id="rId347" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B378" r:id="rId348" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B379" r:id="rId349" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B380" r:id="rId350" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B381" r:id="rId351" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B382" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B383" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B384" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B385" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B386" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B387" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B388" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B389" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B390" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B391" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B393" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B392" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B394" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B395" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B396" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B399" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B400" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B401" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B402" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B403" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B404" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B407" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B408" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B409" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B410" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B411" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B412" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B413" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B414" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B415" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B416" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B417" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B418" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B419" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B420" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B421" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B422" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B423" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B424" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B425" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B426" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B427" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B428" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B429" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B430" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B431" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B432" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B433" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B434" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B435" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B436" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B437" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B438" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B439" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B440" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B441" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B442" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B443" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B444" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B445" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B446" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B448" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B447" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B449" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B450" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B451" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B452" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B453" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B454" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B455" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B456" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B457" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B458" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B459" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B466" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B465" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B464" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B463" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B462" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B461" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B460" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B469" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B470" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B471" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B472" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B473" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B474" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B475" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B478" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B476" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B477" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B353" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B12" r:id="rId444" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
+    <hyperlink ref="B31" r:id="rId445" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId446"/>

</xml_diff>

<commit_message>
Add cpp code for q31-36, completed cpp/Arrays
</commit_message>
<xml_diff>
--- a/Love Babbar 450 DSA Questions/FINAL450.xlsx
+++ b/Love Babbar 450 DSA Questions/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhroov\Desktop\Projects\dsa\Love Babbar 450 DSA Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A48CF2C-20BF-4CC6-986D-316E6351FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FD13EA-A141-4BFF-B5BD-E62B40FB377C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="516">
   <si>
     <t>Topic:</t>
   </si>
@@ -1564,6 +1564,21 @@
   </si>
   <si>
     <t>ChocolateDistribution.cpp</t>
+  </si>
+  <si>
+    <t>SmallestSubarrayWithSumGteX.cpp</t>
+  </si>
+  <si>
+    <t>ThreeWayPartitioning.cpp</t>
+  </si>
+  <si>
+    <t>MinSwapsToBringNumsLteKTogether.cpp</t>
+  </si>
+  <si>
+    <t>MinMergeOpsToMakeArrPalindrome.cpp</t>
+  </si>
+  <si>
+    <t>MedianOfSortedArr.cpp</t>
   </si>
 </sst>
 </file>
@@ -1633,7 +1648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1643,6 +1658,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1660,7 +1681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1687,6 +1708,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2006,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2510,7 +2543,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -2518,10 +2551,13 @@
         <v>34</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -2529,21 +2565,27 @@
         <v>35</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
@@ -2551,10 +2593,13 @@
         <v>37</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -2562,34 +2607,40 @@
         <v>38</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B39" s="3"/>
-      <c r="C39" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>463</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="16"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
@@ -2600,7 +2651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -2611,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>40</v>
       </c>
@@ -2622,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>40</v>
       </c>
@@ -2633,7 +2684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>40</v>
       </c>
@@ -2644,7 +2695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -2655,7 +2706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>40</v>
       </c>
@@ -2677,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
@@ -2688,7 +2739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>40</v>
       </c>
@@ -2699,12 +2750,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="1"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="9"/>
-    </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A52" s="16"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -2715,7 +2773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -2726,7 +2784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -2737,7 +2795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -2748,7 +2806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -2759,7 +2817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
@@ -2770,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>51</v>
       </c>
@@ -2781,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>51</v>
       </c>
@@ -2792,7 +2850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>51</v>
       </c>
@@ -2803,7 +2861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>51</v>
       </c>
@@ -2814,7 +2872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -2825,7 +2883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>51</v>
       </c>
@@ -3012,7 +3070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>51</v>
       </c>
@@ -3023,7 +3081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>51</v>
       </c>
@@ -3034,7 +3092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>51</v>
       </c>
@@ -3045,7 +3103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>51</v>
       </c>
@@ -3056,7 +3114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
@@ -3067,7 +3125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>51</v>
       </c>
@@ -3078,7 +3136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>51</v>
       </c>
@@ -3089,7 +3147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>51</v>
       </c>
@@ -3100,7 +3158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>51</v>
       </c>
@@ -3111,7 +3169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>51</v>
       </c>
@@ -3122,7 +3180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>51</v>
       </c>
@@ -3133,7 +3191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>51</v>
       </c>
@@ -3144,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>51</v>
       </c>
@@ -3155,7 +3213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>51</v>
       </c>
@@ -3166,7 +3224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>51</v>
       </c>
@@ -3177,12 +3235,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A97" s="4"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="9"/>
-    </row>
-    <row r="98" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+    </row>
+    <row r="97" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A97" s="17"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+    </row>
+    <row r="98" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -3193,7 +3258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -3204,7 +3269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -3215,7 +3280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>95</v>
       </c>
@@ -3226,7 +3291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>95</v>
       </c>
@@ -3237,7 +3302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>95</v>
       </c>
@@ -3248,7 +3313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>95</v>
       </c>
@@ -3259,7 +3324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>95</v>
       </c>
@@ -3270,7 +3335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
@@ -3281,7 +3346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>95</v>
       </c>
@@ -3292,7 +3357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>95</v>
       </c>
@@ -3303,7 +3368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>95</v>
       </c>
@@ -3314,7 +3379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>95</v>
       </c>
@@ -3325,7 +3390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>95</v>
       </c>
@@ -3336,7 +3401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>95</v>
       </c>
@@ -3523,7 +3588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>95</v>
       </c>
@@ -3534,7 +3599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>95</v>
       </c>
@@ -3545,7 +3610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>95</v>
       </c>
@@ -3556,7 +3621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>95</v>
       </c>
@@ -3567,7 +3632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>95</v>
       </c>
@@ -3578,11 +3643,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B135" s="3"/>
-      <c r="C135" s="9"/>
-    </row>
-    <row r="136" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+    </row>
+    <row r="135" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B135" s="13"/>
+      <c r="C135" s="14"/>
+      <c r="D135" s="15"/>
+      <c r="E135" s="15"/>
+    </row>
+    <row r="136" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>132</v>
       </c>
@@ -3593,7 +3665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>132</v>
       </c>
@@ -3604,7 +3676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>132</v>
       </c>
@@ -3615,7 +3687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>132</v>
       </c>
@@ -3626,7 +3698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>132</v>
       </c>
@@ -3637,7 +3709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>132</v>
       </c>
@@ -3648,7 +3720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>132</v>
       </c>
@@ -3659,7 +3731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
         <v>132</v>
       </c>
@@ -3670,7 +3742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
         <v>132</v>
       </c>
@@ -3857,7 +3929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
         <v>132</v>
       </c>
@@ -3868,7 +3940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
         <v>132</v>
       </c>
@@ -3879,7 +3951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>132</v>
       </c>
@@ -3890,7 +3962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
         <v>132</v>
       </c>
@@ -3901,7 +3973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
         <v>132</v>
       </c>
@@ -3912,7 +3984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
         <v>132</v>
       </c>
@@ -3923,7 +3995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
         <v>132</v>
       </c>
@@ -3934,7 +4006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
         <v>132</v>
       </c>
@@ -3945,7 +4017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
         <v>132</v>
       </c>
@@ -3956,7 +4028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
         <v>132</v>
       </c>
@@ -3967,7 +4039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
         <v>132</v>
       </c>
@@ -3978,11 +4050,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B173" s="3"/>
-      <c r="C173" s="9"/>
-    </row>
-    <row r="174" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="E172" s="15"/>
+    </row>
+    <row r="173" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B173" s="13"/>
+      <c r="C173" s="14"/>
+      <c r="D173" s="15"/>
+      <c r="E173" s="15"/>
+    </row>
+    <row r="174" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>169</v>
       </c>
@@ -3993,7 +4072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>169</v>
       </c>
@@ -4004,7 +4083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>169</v>
       </c>
@@ -4367,17 +4446,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A209" s="4"/>
-      <c r="B209" s="3"/>
-      <c r="C209" s="9"/>
-    </row>
-    <row r="210" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A210" s="4"/>
-      <c r="B210" s="3"/>
-      <c r="C210" s="9"/>
-    </row>
-    <row r="211" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A209" s="17"/>
+      <c r="B209" s="13"/>
+      <c r="C209" s="14"/>
+      <c r="D209" s="15"/>
+      <c r="E209" s="15"/>
+    </row>
+    <row r="210" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A210" s="17"/>
+      <c r="B210" s="13"/>
+      <c r="C210" s="14"/>
+      <c r="D210" s="15"/>
+      <c r="E210" s="15"/>
+    </row>
+    <row r="211" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>205</v>
       </c>
@@ -4388,7 +4471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>205</v>
       </c>
@@ -4399,7 +4482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>205</v>
       </c>
@@ -4410,7 +4493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>205</v>
       </c>
@@ -4421,7 +4504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>205</v>
       </c>
@@ -4432,7 +4515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>205</v>
       </c>
@@ -4443,7 +4526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>205</v>
       </c>
@@ -4454,7 +4537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>205</v>
       </c>
@@ -4465,7 +4548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>205</v>
       </c>
@@ -4476,7 +4559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>205</v>
       </c>
@@ -4487,7 +4570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>205</v>
       </c>
@@ -4498,7 +4581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>205</v>
       </c>
@@ -4509,7 +4592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>205</v>
       </c>
@@ -4520,7 +4603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>205</v>
       </c>
@@ -4531,7 +4614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>205</v>
       </c>
@@ -4542,7 +4625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>205</v>
       </c>
@@ -4553,7 +4636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>205</v>
       </c>
@@ -4564,7 +4647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>205</v>
       </c>
@@ -4575,7 +4658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>205</v>
       </c>
@@ -4586,7 +4669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>205</v>
       </c>
@@ -4597,7 +4680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>205</v>
       </c>
@@ -4608,7 +4691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A232" s="1" t="s">
         <v>205</v>
       </c>
@@ -4619,15 +4702,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B233" s="3"/>
-      <c r="C233" s="9"/>
-    </row>
-    <row r="234" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B234" s="3"/>
-      <c r="C234" s="9"/>
-    </row>
-    <row r="235" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B233" s="13"/>
+      <c r="C233" s="14"/>
+      <c r="D233" s="15"/>
+      <c r="E233" s="15"/>
+    </row>
+    <row r="234" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B234" s="13"/>
+      <c r="C234" s="14"/>
+      <c r="D234" s="15"/>
+      <c r="E234" s="15"/>
+    </row>
+    <row r="235" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>228</v>
       </c>
@@ -4638,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>228</v>
       </c>
@@ -4649,7 +4736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>228</v>
       </c>
@@ -4660,7 +4747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>228</v>
       </c>
@@ -4671,7 +4758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A239" s="1" t="s">
         <v>228</v>
       </c>
@@ -4682,7 +4769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A240" s="1" t="s">
         <v>228</v>
       </c>
@@ -4869,7 +4956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>228</v>
       </c>
@@ -4880,7 +4967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A258" s="1" t="s">
         <v>228</v>
       </c>
@@ -4891,7 +4978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>228</v>
       </c>
@@ -4902,7 +4989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>228</v>
       </c>
@@ -4913,7 +5000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>228</v>
       </c>
@@ -4924,7 +5011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>228</v>
       </c>
@@ -4935,7 +5022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>228</v>
       </c>
@@ -4946,7 +5033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
         <v>228</v>
       </c>
@@ -4957,7 +5044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="265" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
         <v>228</v>
       </c>
@@ -4968,7 +5055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
         <v>228</v>
       </c>
@@ -4979,7 +5066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
         <v>228</v>
       </c>
@@ -4990,7 +5077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
         <v>228</v>
       </c>
@@ -5001,7 +5088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="269" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A269" s="1" t="s">
         <v>228</v>
       </c>
@@ -5012,15 +5099,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="270" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B270" s="3"/>
-      <c r="C270" s="9"/>
-    </row>
-    <row r="271" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B271" s="3"/>
-      <c r="C271" s="9"/>
-    </row>
-    <row r="272" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B270" s="13"/>
+      <c r="C270" s="14"/>
+      <c r="D270" s="15"/>
+      <c r="E270" s="15"/>
+    </row>
+    <row r="271" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B271" s="13"/>
+      <c r="C271" s="14"/>
+      <c r="D271" s="15"/>
+      <c r="E271" s="15"/>
+    </row>
+    <row r="272" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
         <v>263</v>
       </c>
@@ -5207,7 +5298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A289" s="1" t="s">
         <v>263</v>
       </c>
@@ -5218,7 +5309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A290" s="1" t="s">
         <v>263</v>
       </c>
@@ -5229,15 +5320,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B291" s="3"/>
-      <c r="C291" s="9"/>
-    </row>
-    <row r="292" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B292" s="3"/>
-      <c r="C292" s="9"/>
-    </row>
-    <row r="293" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B291" s="13"/>
+      <c r="C291" s="14"/>
+      <c r="D291" s="15"/>
+      <c r="E291" s="15"/>
+    </row>
+    <row r="292" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B292" s="13"/>
+      <c r="C292" s="14"/>
+      <c r="D292" s="15"/>
+      <c r="E292" s="15"/>
+    </row>
+    <row r="293" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A293" s="1" t="s">
         <v>283</v>
       </c>
@@ -5248,7 +5343,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A294" s="1" t="s">
         <v>283</v>
       </c>
@@ -5259,7 +5354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A295" s="1" t="s">
         <v>283</v>
       </c>
@@ -5270,7 +5365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A296" s="1" t="s">
         <v>283</v>
       </c>
@@ -5281,7 +5376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="297" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A297" s="1" t="s">
         <v>283</v>
       </c>
@@ -5292,7 +5387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A298" s="1" t="s">
         <v>283</v>
       </c>
@@ -5303,7 +5398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A299" s="1" t="s">
         <v>283</v>
       </c>
@@ -5314,7 +5409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A300" s="1" t="s">
         <v>283</v>
       </c>
@@ -5325,7 +5420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A301" s="1" t="s">
         <v>283</v>
       </c>
@@ -5336,7 +5431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A302" s="1" t="s">
         <v>283</v>
       </c>
@@ -5347,7 +5442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A303" s="1" t="s">
         <v>283</v>
       </c>
@@ -5358,7 +5453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="304" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A304" s="1" t="s">
         <v>283</v>
       </c>
@@ -5545,7 +5640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A321" s="1" t="s">
         <v>283</v>
       </c>
@@ -5556,7 +5651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A322" s="1" t="s">
         <v>283</v>
       </c>
@@ -5567,7 +5662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="323" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
         <v>283</v>
       </c>
@@ -5578,7 +5673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A324" s="1" t="s">
         <v>283</v>
       </c>
@@ -5589,7 +5684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A325" s="1" t="s">
         <v>283</v>
       </c>
@@ -5600,7 +5695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A326" s="1" t="s">
         <v>283</v>
       </c>
@@ -5611,7 +5706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A327" s="1" t="s">
         <v>283</v>
       </c>
@@ -5622,7 +5717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A328" s="1" t="s">
         <v>283</v>
       </c>
@@ -5633,7 +5728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="329" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A329" s="1" t="s">
         <v>283</v>
       </c>
@@ -5644,7 +5739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A330" s="1" t="s">
         <v>283</v>
       </c>
@@ -5655,15 +5750,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B331" s="3"/>
-      <c r="C331" s="9"/>
-    </row>
-    <row r="332" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B332" s="3"/>
-      <c r="C332" s="9"/>
-    </row>
-    <row r="333" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B331" s="13"/>
+      <c r="C331" s="14"/>
+      <c r="D331" s="15"/>
+      <c r="E331" s="15"/>
+    </row>
+    <row r="332" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B332" s="13"/>
+      <c r="C332" s="14"/>
+      <c r="D332" s="15"/>
+      <c r="E332" s="15"/>
+    </row>
+    <row r="333" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A333" s="4" t="s">
         <v>322</v>
       </c>
@@ -5674,7 +5773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A334" s="4" t="s">
         <v>322</v>
       </c>
@@ -5685,7 +5784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="335" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A335" s="4" t="s">
         <v>322</v>
       </c>
@@ -5696,7 +5795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A336" s="4" t="s">
         <v>322</v>
       </c>
@@ -5707,7 +5806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A337" s="4" t="s">
         <v>322</v>
       </c>
@@ -5718,7 +5817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="338" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A338" s="4" t="s">
         <v>322</v>
       </c>
@@ -5729,7 +5828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A339" s="4" t="s">
         <v>322</v>
       </c>
@@ -5740,7 +5839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A340" s="4" t="s">
         <v>322</v>
       </c>
@@ -5751,7 +5850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A341" s="4" t="s">
         <v>322</v>
       </c>
@@ -5762,7 +5861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A342" s="4" t="s">
         <v>322</v>
       </c>
@@ -5773,7 +5872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="343" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A343" s="4" t="s">
         <v>322</v>
       </c>
@@ -5784,7 +5883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A344" s="4" t="s">
         <v>322</v>
       </c>
@@ -5795,7 +5894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A345" s="4" t="s">
         <v>322</v>
       </c>
@@ -5806,7 +5905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A346" s="4" t="s">
         <v>322</v>
       </c>
@@ -5817,7 +5916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A347" s="4" t="s">
         <v>322</v>
       </c>
@@ -5828,7 +5927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A348" s="4" t="s">
         <v>322</v>
       </c>
@@ -5839,7 +5938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A349" s="4" t="s">
         <v>322</v>
       </c>
@@ -5850,7 +5949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A350" s="4" t="s">
         <v>322</v>
       </c>
@@ -5861,13 +5960,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B351" s="3"/>
-      <c r="C351" s="9"/>
-    </row>
-    <row r="352" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B352" s="3"/>
-      <c r="C352" s="9"/>
+    <row r="351" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B351" s="13"/>
+      <c r="C351" s="14"/>
+      <c r="D351" s="15"/>
+      <c r="E351" s="15"/>
+    </row>
+    <row r="352" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B352" s="13"/>
+      <c r="C352" s="14"/>
+      <c r="D352" s="15"/>
+      <c r="E352" s="15"/>
     </row>
     <row r="353" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A353" s="4" t="s">
@@ -6221,7 +6324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A385" s="4" t="s">
         <v>341</v>
       </c>
@@ -6232,7 +6335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A386" s="4" t="s">
         <v>341</v>
       </c>
@@ -6243,7 +6346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A387" s="4" t="s">
         <v>341</v>
       </c>
@@ -6254,7 +6357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A388" s="4" t="s">
         <v>341</v>
       </c>
@@ -6265,7 +6368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A389" s="4" t="s">
         <v>341</v>
       </c>
@@ -6276,7 +6379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A390" s="4" t="s">
         <v>341</v>
       </c>
@@ -6287,7 +6390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A391" s="4" t="s">
         <v>341</v>
       </c>
@@ -6298,7 +6401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A392" s="4" t="s">
         <v>341</v>
       </c>
@@ -6309,7 +6412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A393" s="4" t="s">
         <v>341</v>
       </c>
@@ -6320,7 +6423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A394" s="4" t="s">
         <v>341</v>
       </c>
@@ -6331,7 +6434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A395" s="4" t="s">
         <v>341</v>
       </c>
@@ -6342,7 +6445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A396" s="4" t="s">
         <v>341</v>
       </c>
@@ -6353,15 +6456,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B397" s="3"/>
-      <c r="C397" s="9"/>
-    </row>
-    <row r="398" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B398" s="3"/>
-      <c r="C398" s="9"/>
-    </row>
-    <row r="399" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B397" s="13"/>
+      <c r="C397" s="14"/>
+      <c r="D397" s="15"/>
+      <c r="E397" s="15"/>
+    </row>
+    <row r="398" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B398" s="13"/>
+      <c r="C398" s="14"/>
+      <c r="D398" s="15"/>
+      <c r="E398" s="15"/>
+    </row>
+    <row r="399" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A399" s="4" t="s">
         <v>385</v>
       </c>
@@ -6372,7 +6479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A400" s="4" t="s">
         <v>385</v>
       </c>
@@ -6383,7 +6490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="401" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A401" s="4" t="s">
         <v>385</v>
       </c>
@@ -6394,7 +6501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="402" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A402" s="4" t="s">
         <v>385</v>
       </c>
@@ -6405,7 +6512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="403" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A403" s="4" t="s">
         <v>385</v>
       </c>
@@ -6416,7 +6523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A404" s="4" t="s">
         <v>385</v>
       </c>
@@ -6427,15 +6534,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="405" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B405" s="3"/>
-      <c r="C405" s="9"/>
-    </row>
-    <row r="406" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B406" s="3"/>
-      <c r="C406" s="9"/>
-    </row>
-    <row r="407" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B405" s="13"/>
+      <c r="C405" s="14"/>
+      <c r="D405" s="15"/>
+      <c r="E405" s="15"/>
+    </row>
+    <row r="406" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B406" s="13"/>
+      <c r="C406" s="14"/>
+      <c r="D406" s="15"/>
+      <c r="E406" s="15"/>
+    </row>
+    <row r="407" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A407" s="1" t="s">
         <v>391</v>
       </c>
@@ -6446,7 +6557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="408" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A408" s="1" t="s">
         <v>391</v>
       </c>
@@ -6457,7 +6568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="409" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A409" s="1" t="s">
         <v>391</v>
       </c>
@@ -6468,7 +6579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="410" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A410" s="1" t="s">
         <v>391</v>
       </c>
@@ -6479,7 +6590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A411" s="1" t="s">
         <v>391</v>
       </c>
@@ -6490,7 +6601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A412" s="1" t="s">
         <v>391</v>
       </c>
@@ -6501,7 +6612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A413" s="1" t="s">
         <v>391</v>
       </c>
@@ -6512,7 +6623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="414" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A414" s="1" t="s">
         <v>391</v>
       </c>
@@ -6523,7 +6634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="415" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A415" s="1" t="s">
         <v>391</v>
       </c>
@@ -6534,7 +6645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="416" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A416" s="1" t="s">
         <v>391</v>
       </c>
@@ -7073,7 +7184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="465" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A465" s="1" t="s">
         <v>391</v>
       </c>
@@ -7084,7 +7195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="466" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A466" s="1" t="s">
         <v>391</v>
       </c>
@@ -7095,16 +7206,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="467" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B467" s="3"/>
-      <c r="C467" s="9"/>
-    </row>
-    <row r="468" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A468" s="4"/>
-      <c r="B468" s="3"/>
-      <c r="C468" s="9"/>
-    </row>
-    <row r="469" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B467" s="13"/>
+      <c r="C467" s="14"/>
+      <c r="D467" s="15"/>
+      <c r="E467" s="15"/>
+    </row>
+    <row r="468" spans="1:5" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A468" s="17"/>
+      <c r="B468" s="13"/>
+      <c r="C468" s="14"/>
+      <c r="D468" s="15"/>
+      <c r="E468" s="15"/>
+    </row>
+    <row r="469" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A469" s="1" t="s">
         <v>451</v>
       </c>
@@ -7115,7 +7230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="470" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A470" s="1" t="s">
         <v>451</v>
       </c>
@@ -7126,7 +7241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="471" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A471" s="1" t="s">
         <v>451</v>
       </c>
@@ -7137,7 +7252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="472" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A472" s="1" t="s">
         <v>451</v>
       </c>
@@ -7148,7 +7263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="473" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A473" s="1" t="s">
         <v>451</v>
       </c>
@@ -7159,7 +7274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="474" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A474" s="1" t="s">
         <v>451</v>
       </c>
@@ -7170,7 +7285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="475" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A475" s="1" t="s">
         <v>451</v>
       </c>
@@ -7181,7 +7296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="476" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A476" s="1" t="s">
         <v>451</v>
       </c>
@@ -7192,7 +7307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="477" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A477" s="1" t="s">
         <v>451</v>
       </c>
@@ -7203,7 +7318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="478" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A478" s="1" t="s">
         <v>451</v>
       </c>
@@ -7247,420 +7362,420 @@
     <hyperlink ref="B33" r:id="rId29" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
     <hyperlink ref="B34" r:id="rId30" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
     <hyperlink ref="B35" r:id="rId31" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="B36" r:id="rId32" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="B37" r:id="rId33" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="B38" r:id="rId34" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
-    <hyperlink ref="B41" r:id="rId35" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
-    <hyperlink ref="B42" r:id="rId36" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="B43" r:id="rId37" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="B44" r:id="rId38" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="B45" r:id="rId39" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="B46" r:id="rId40" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="B47" r:id="rId41" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="B48" r:id="rId42" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="B49" r:id="rId43" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="B50" r:id="rId44" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="B53" r:id="rId45" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="B54" r:id="rId46" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
-    <hyperlink ref="B55" r:id="rId47" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
-    <hyperlink ref="B57" r:id="rId48" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
-    <hyperlink ref="B58" r:id="rId49" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
-    <hyperlink ref="B59" r:id="rId50" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
-    <hyperlink ref="B60" r:id="rId51" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
-    <hyperlink ref="B61" r:id="rId52" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
-    <hyperlink ref="B62" r:id="rId53" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
-    <hyperlink ref="B63" r:id="rId54" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
-    <hyperlink ref="B64" r:id="rId55" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
-    <hyperlink ref="B65" r:id="rId56" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
-    <hyperlink ref="B66" r:id="rId57" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
-    <hyperlink ref="B67" r:id="rId58" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
-    <hyperlink ref="B68" r:id="rId59" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
-    <hyperlink ref="B69" r:id="rId60" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
-    <hyperlink ref="B70" r:id="rId61" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
-    <hyperlink ref="B71" r:id="rId62" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
-    <hyperlink ref="B72" r:id="rId63" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
-    <hyperlink ref="B73" r:id="rId64" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
-    <hyperlink ref="B74" r:id="rId65" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
-    <hyperlink ref="B75" r:id="rId66" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
-    <hyperlink ref="B76" r:id="rId67" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
-    <hyperlink ref="B77" r:id="rId68" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
-    <hyperlink ref="B78" r:id="rId69" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
-    <hyperlink ref="B79" r:id="rId70" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
-    <hyperlink ref="B80" r:id="rId71" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
-    <hyperlink ref="B81" r:id="rId72" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
-    <hyperlink ref="B82" r:id="rId73" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
-    <hyperlink ref="B83" r:id="rId74" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="B84" r:id="rId75" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="B85" r:id="rId76" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="B86" r:id="rId77" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="B87" r:id="rId78" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="B88" r:id="rId79" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="B89" r:id="rId80" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="B90" r:id="rId81" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="B91" r:id="rId82" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="B92" r:id="rId83" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="B93" r:id="rId84" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="B94" r:id="rId85" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="B95" r:id="rId86" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="B98" r:id="rId87" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="B99" r:id="rId88" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="B100" r:id="rId89" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="B101" r:id="rId90" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="B103" r:id="rId91" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="B104" r:id="rId92" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="B105" r:id="rId93" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="B106" r:id="rId94" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="B107" r:id="rId95" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="B108" r:id="rId96" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="B110" r:id="rId97" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="B111" r:id="rId98" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="B112" r:id="rId99" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="B113" r:id="rId100" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="B114" r:id="rId101" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="B115" r:id="rId102" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="B116" r:id="rId103" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="B117" r:id="rId104" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="B118" r:id="rId105" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="B119" r:id="rId106" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="B120" r:id="rId107" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="B121" r:id="rId108" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="B122" r:id="rId109" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="B123" r:id="rId110" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="B124" r:id="rId111" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="B125" r:id="rId112" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="B126" r:id="rId113" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="B127" r:id="rId114" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="B128" r:id="rId115" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="B129" r:id="rId116" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="B130" r:id="rId117" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="B131" r:id="rId118" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="B132" r:id="rId119" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="B133" r:id="rId120" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="B102" r:id="rId121" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="B109" r:id="rId122" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="B136" r:id="rId123" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="B137" r:id="rId124" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="B138" r:id="rId125" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="B139" r:id="rId126" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="B140" r:id="rId127" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="B141" r:id="rId128" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="B142" r:id="rId129" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="B143" r:id="rId130" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="B144" r:id="rId131" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="B145" r:id="rId132" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="B146" r:id="rId133" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="B147" r:id="rId134" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="B148" r:id="rId135" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="B149" r:id="rId136" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="B150" r:id="rId137" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="B151" r:id="rId138" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="B152" r:id="rId139" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="B153" r:id="rId140" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="B154" r:id="rId141" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="B155" r:id="rId142" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="B156" r:id="rId143" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="B157" r:id="rId144" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="B158" r:id="rId145" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="B159" r:id="rId146" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="B160" r:id="rId147" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="B163" r:id="rId148" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="B164" r:id="rId149" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="B165" r:id="rId150" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="B166" r:id="rId151" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="B167" r:id="rId152" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="B168" r:id="rId153" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="B169" r:id="rId154" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="B170" r:id="rId155" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="B171" r:id="rId156" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="B174" r:id="rId157" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="B175" r:id="rId158" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="B176" r:id="rId159" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="B177" r:id="rId160" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="B178" r:id="rId161" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="B179" r:id="rId162" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="B180" r:id="rId163" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="B181" r:id="rId164" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="B182" r:id="rId165" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="B183" r:id="rId166" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="B184" r:id="rId167" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="B185" r:id="rId168" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="B186" r:id="rId169" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="B187" r:id="rId170" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="B188" r:id="rId171" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="B189" r:id="rId172" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="B190" r:id="rId173" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="B191" r:id="rId174" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="B192" r:id="rId175" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="B193" r:id="rId176" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="B194" r:id="rId177" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="B195" r:id="rId178" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="B196" r:id="rId179" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="B197" r:id="rId180" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="B198" r:id="rId181" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="B199" r:id="rId182" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="B200" r:id="rId183" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="B201" r:id="rId184" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="B202" r:id="rId185" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="B203" r:id="rId186" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="B204" r:id="rId187" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="B205" r:id="rId188" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="B206" r:id="rId189" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="B207" r:id="rId190" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="B208" r:id="rId191" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="B211" r:id="rId192" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="B212" r:id="rId193" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="B213" r:id="rId194" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="B214" r:id="rId195" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="B215" r:id="rId196" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="B216" r:id="rId197" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="B217" r:id="rId198" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="B218" r:id="rId199" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="B219" r:id="rId200" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="B220" r:id="rId201" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="B221" r:id="rId202" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="B222" r:id="rId203" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="B223" r:id="rId204" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="B224" r:id="rId205" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="B225" r:id="rId206" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="B226" r:id="rId207" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="B227" r:id="rId208" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="B228" r:id="rId209" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="B229" r:id="rId210" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="B230" r:id="rId211" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="B231" r:id="rId212" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="B232" r:id="rId213" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="B235" r:id="rId214" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="B236" r:id="rId215" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="B237" r:id="rId216" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="B238" r:id="rId217" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="B239" r:id="rId218" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="B240" r:id="rId219" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="B241" r:id="rId220" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="B242" r:id="rId221" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="B243" r:id="rId222" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="B244" r:id="rId223" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="B245" r:id="rId224" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="B246" r:id="rId225" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="B247" r:id="rId226" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="B248" r:id="rId227" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="B249" r:id="rId228" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="B250" r:id="rId229" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="B251" r:id="rId230" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="B252" r:id="rId231" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="B253" r:id="rId232" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="B254" r:id="rId233" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="B255" r:id="rId234" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="B256" r:id="rId235" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="B257" r:id="rId236" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="B258" r:id="rId237" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="B259" r:id="rId238" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="B260" r:id="rId239" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="B261" r:id="rId240" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="B262" r:id="rId241" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="B263" r:id="rId242" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="B264" r:id="rId243" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="B265" r:id="rId244" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="B266" r:id="rId245" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="B267" r:id="rId246" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="B268" r:id="rId247" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="B269" r:id="rId248" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="B272" r:id="rId249" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="B273" r:id="rId250" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="B274" r:id="rId251" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="B275" r:id="rId252" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="B276" r:id="rId253" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="B277" r:id="rId254" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="B278" r:id="rId255" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="B279" r:id="rId256" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="B280" r:id="rId257" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="B281" r:id="rId258" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="B282" r:id="rId259" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="B283" r:id="rId260" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="B284" r:id="rId261" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="B285" r:id="rId262" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="B286" r:id="rId263" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="B287" r:id="rId264" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="B288" r:id="rId265" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="B289" r:id="rId266" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="B290" r:id="rId267" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="B293" r:id="rId268" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="B294" r:id="rId269" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="B295" r:id="rId270" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="B296" r:id="rId271" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="B297" r:id="rId272" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="B298" r:id="rId273" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="B299" r:id="rId274" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="B300" r:id="rId275" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="B301" r:id="rId276" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="B302" r:id="rId277" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="B303" r:id="rId278" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="B304" r:id="rId279" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="B305" r:id="rId280" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="B306" r:id="rId281" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="B307" r:id="rId282" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="B308" r:id="rId283" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="B309" r:id="rId284" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="B310" r:id="rId285" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="B311" r:id="rId286" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="B312" r:id="rId287" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="B313" r:id="rId288" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="B314" r:id="rId289" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="B315" r:id="rId290" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="B316" r:id="rId291" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="B317" r:id="rId292" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="B318" r:id="rId293" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="B319" r:id="rId294" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="B320" r:id="rId295" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="B321" r:id="rId296" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="B322" r:id="rId297" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="B323" r:id="rId298" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="B324" r:id="rId299" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="B325" r:id="rId300" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="B326" r:id="rId301" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="B327" r:id="rId302" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="B328" r:id="rId303" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="B329" r:id="rId304" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="B330" r:id="rId305" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="B333" r:id="rId306" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="B334" r:id="rId307" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="B335" r:id="rId308" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="B336" r:id="rId309" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="B337" r:id="rId310" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="B338" r:id="rId311" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="B339" r:id="rId312" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="B340" r:id="rId313" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="B341" r:id="rId314" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="B342" r:id="rId315" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="B343" r:id="rId316" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="B344" r:id="rId317" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="B345" r:id="rId318" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="B346" r:id="rId319" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="B347" r:id="rId320" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="B348" r:id="rId321" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="B349" r:id="rId322" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="B350" r:id="rId323" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="B354" r:id="rId324" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="B355" r:id="rId325" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="B356" r:id="rId326" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="B357" r:id="rId327" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="B358" r:id="rId328" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="B359" r:id="rId329" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="B360" r:id="rId330" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="B361" r:id="rId331" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="B362" r:id="rId332" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="B363" r:id="rId333" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="B364" r:id="rId334" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="B365" r:id="rId335" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="B366" r:id="rId336" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="B367" r:id="rId337" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="B368" r:id="rId338" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="B369" r:id="rId339" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="B370" r:id="rId340" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="B371" r:id="rId341" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="B372" r:id="rId342" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="B373" r:id="rId343" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="B374" r:id="rId344" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="B375" r:id="rId345" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="B376" r:id="rId346" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="B377" r:id="rId347" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="B378" r:id="rId348" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="B379" r:id="rId349" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="B380" r:id="rId350" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="B381" r:id="rId351" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="B382" r:id="rId352" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="B383" r:id="rId353" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="B384" r:id="rId354" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="B385" r:id="rId355" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="B386" r:id="rId356" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="B387" r:id="rId357" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="B388" r:id="rId358" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="B389" r:id="rId359" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="B390" r:id="rId360" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="B391" r:id="rId361" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="B393" r:id="rId362" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="B392" r:id="rId363" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="B394" r:id="rId364" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="B395" r:id="rId365" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="B396" r:id="rId366" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="B399" r:id="rId367" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="B400" r:id="rId368" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="B401" r:id="rId369" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="B402" r:id="rId370" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="B403" r:id="rId371" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="B404" r:id="rId372" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="B407" r:id="rId373" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="B408" r:id="rId374" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="B409" r:id="rId375" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="B410" r:id="rId376" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="B411" r:id="rId377" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="B412" r:id="rId378" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="B413" r:id="rId379" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="B414" r:id="rId380" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="B415" r:id="rId381" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="B416" r:id="rId382" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="B417" r:id="rId383" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="B418" r:id="rId384" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="B419" r:id="rId385" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="B420" r:id="rId386" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="B421" r:id="rId387" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="B422" r:id="rId388" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="B423" r:id="rId389" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="B424" r:id="rId390" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="B425" r:id="rId391" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="B426" r:id="rId392" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="B427" r:id="rId393" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="B428" r:id="rId394" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="B429" r:id="rId395" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="B430" r:id="rId396" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="B431" r:id="rId397" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="B432" r:id="rId398" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="B433" r:id="rId399" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="B434" r:id="rId400" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="B435" r:id="rId401" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="B436" r:id="rId402" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="B437" r:id="rId403" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="B438" r:id="rId404" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="B439" r:id="rId405" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="B440" r:id="rId406" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="B441" r:id="rId407" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="B442" r:id="rId408" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="B443" r:id="rId409" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="B444" r:id="rId410" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="B445" r:id="rId411" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="B446" r:id="rId412" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="B448" r:id="rId413" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="B447" r:id="rId414" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="B449" r:id="rId415" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="B450" r:id="rId416" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="B451" r:id="rId417" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="B452" r:id="rId418" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="B453" r:id="rId419" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="B454" r:id="rId420" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="B455" r:id="rId421" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="B456" r:id="rId422" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="B457" r:id="rId423" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="B458" r:id="rId424" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="B459" r:id="rId425" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="B466" r:id="rId426" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="B465" r:id="rId427" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="B464" r:id="rId428" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="B463" r:id="rId429" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="B462" r:id="rId430" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="B461" r:id="rId431" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="B460" r:id="rId432" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="B469" r:id="rId433" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="B470" r:id="rId434" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="B471" r:id="rId435" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="B472" r:id="rId436" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="B473" r:id="rId437" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="B474" r:id="rId438" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="B475" r:id="rId439" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="B478" r:id="rId440" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="B476" r:id="rId441" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="B477" r:id="rId442" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="B353" r:id="rId443" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="B12" r:id="rId444" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
-    <hyperlink ref="B31" r:id="rId445" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
+    <hyperlink ref="B37" r:id="rId32" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
+    <hyperlink ref="B41" r:id="rId34" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
+    <hyperlink ref="B42" r:id="rId35" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
+    <hyperlink ref="B43" r:id="rId36" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
+    <hyperlink ref="B44" r:id="rId37" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
+    <hyperlink ref="B45" r:id="rId38" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
+    <hyperlink ref="B46" r:id="rId39" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
+    <hyperlink ref="B47" r:id="rId40" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
+    <hyperlink ref="B48" r:id="rId41" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
+    <hyperlink ref="B49" r:id="rId42" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
+    <hyperlink ref="B50" r:id="rId43" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
+    <hyperlink ref="B53" r:id="rId44" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
+    <hyperlink ref="B54" r:id="rId45" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
+    <hyperlink ref="B55" r:id="rId46" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
+    <hyperlink ref="B57" r:id="rId47" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
+    <hyperlink ref="B58" r:id="rId48" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
+    <hyperlink ref="B59" r:id="rId49" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
+    <hyperlink ref="B60" r:id="rId50" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
+    <hyperlink ref="B61" r:id="rId51" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
+    <hyperlink ref="B62" r:id="rId52" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
+    <hyperlink ref="B63" r:id="rId53" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
+    <hyperlink ref="B64" r:id="rId54" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
+    <hyperlink ref="B65" r:id="rId55" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
+    <hyperlink ref="B66" r:id="rId56" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
+    <hyperlink ref="B67" r:id="rId57" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
+    <hyperlink ref="B68" r:id="rId58" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
+    <hyperlink ref="B69" r:id="rId59" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
+    <hyperlink ref="B70" r:id="rId60" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
+    <hyperlink ref="B71" r:id="rId61" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
+    <hyperlink ref="B72" r:id="rId62" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
+    <hyperlink ref="B73" r:id="rId63" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
+    <hyperlink ref="B74" r:id="rId64" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
+    <hyperlink ref="B75" r:id="rId65" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
+    <hyperlink ref="B76" r:id="rId66" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
+    <hyperlink ref="B77" r:id="rId67" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
+    <hyperlink ref="B78" r:id="rId68" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
+    <hyperlink ref="B79" r:id="rId69" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
+    <hyperlink ref="B80" r:id="rId70" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
+    <hyperlink ref="B81" r:id="rId71" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
+    <hyperlink ref="B82" r:id="rId72" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
+    <hyperlink ref="B83" r:id="rId73" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
+    <hyperlink ref="B84" r:id="rId74" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
+    <hyperlink ref="B85" r:id="rId75" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
+    <hyperlink ref="B86" r:id="rId76" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
+    <hyperlink ref="B87" r:id="rId77" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
+    <hyperlink ref="B88" r:id="rId78" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
+    <hyperlink ref="B89" r:id="rId79" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
+    <hyperlink ref="B90" r:id="rId80" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
+    <hyperlink ref="B91" r:id="rId81" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
+    <hyperlink ref="B92" r:id="rId82" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
+    <hyperlink ref="B93" r:id="rId83" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
+    <hyperlink ref="B94" r:id="rId84" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
+    <hyperlink ref="B95" r:id="rId85" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
+    <hyperlink ref="B98" r:id="rId86" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
+    <hyperlink ref="B99" r:id="rId87" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
+    <hyperlink ref="B100" r:id="rId88" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
+    <hyperlink ref="B101" r:id="rId89" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
+    <hyperlink ref="B103" r:id="rId90" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
+    <hyperlink ref="B104" r:id="rId91" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
+    <hyperlink ref="B105" r:id="rId92" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
+    <hyperlink ref="B106" r:id="rId93" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
+    <hyperlink ref="B107" r:id="rId94" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
+    <hyperlink ref="B108" r:id="rId95" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
+    <hyperlink ref="B110" r:id="rId96" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
+    <hyperlink ref="B111" r:id="rId97" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
+    <hyperlink ref="B112" r:id="rId98" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
+    <hyperlink ref="B113" r:id="rId99" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
+    <hyperlink ref="B114" r:id="rId100" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
+    <hyperlink ref="B115" r:id="rId101" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
+    <hyperlink ref="B116" r:id="rId102" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
+    <hyperlink ref="B117" r:id="rId103" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
+    <hyperlink ref="B118" r:id="rId104" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
+    <hyperlink ref="B119" r:id="rId105" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
+    <hyperlink ref="B120" r:id="rId106" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
+    <hyperlink ref="B121" r:id="rId107" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
+    <hyperlink ref="B122" r:id="rId108" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
+    <hyperlink ref="B123" r:id="rId109" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
+    <hyperlink ref="B124" r:id="rId110" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
+    <hyperlink ref="B125" r:id="rId111" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
+    <hyperlink ref="B126" r:id="rId112" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
+    <hyperlink ref="B127" r:id="rId113" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
+    <hyperlink ref="B128" r:id="rId114" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
+    <hyperlink ref="B129" r:id="rId115" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
+    <hyperlink ref="B130" r:id="rId116" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
+    <hyperlink ref="B131" r:id="rId117" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
+    <hyperlink ref="B132" r:id="rId118" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
+    <hyperlink ref="B133" r:id="rId119" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
+    <hyperlink ref="B102" r:id="rId120" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
+    <hyperlink ref="B109" r:id="rId121" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
+    <hyperlink ref="B136" r:id="rId122" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
+    <hyperlink ref="B137" r:id="rId123" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
+    <hyperlink ref="B138" r:id="rId124" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
+    <hyperlink ref="B139" r:id="rId125" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
+    <hyperlink ref="B140" r:id="rId126" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
+    <hyperlink ref="B141" r:id="rId127" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
+    <hyperlink ref="B142" r:id="rId128" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
+    <hyperlink ref="B143" r:id="rId129" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
+    <hyperlink ref="B144" r:id="rId130" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
+    <hyperlink ref="B145" r:id="rId131" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
+    <hyperlink ref="B146" r:id="rId132" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
+    <hyperlink ref="B147" r:id="rId133" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
+    <hyperlink ref="B148" r:id="rId134" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
+    <hyperlink ref="B149" r:id="rId135" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
+    <hyperlink ref="B150" r:id="rId136" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
+    <hyperlink ref="B151" r:id="rId137" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
+    <hyperlink ref="B152" r:id="rId138" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
+    <hyperlink ref="B153" r:id="rId139" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
+    <hyperlink ref="B154" r:id="rId140" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
+    <hyperlink ref="B155" r:id="rId141" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
+    <hyperlink ref="B156" r:id="rId142" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
+    <hyperlink ref="B157" r:id="rId143" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
+    <hyperlink ref="B158" r:id="rId144" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
+    <hyperlink ref="B159" r:id="rId145" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
+    <hyperlink ref="B160" r:id="rId146" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
+    <hyperlink ref="B163" r:id="rId147" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
+    <hyperlink ref="B164" r:id="rId148" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
+    <hyperlink ref="B165" r:id="rId149" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="B166" r:id="rId150" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="B167" r:id="rId151" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
+    <hyperlink ref="B168" r:id="rId152" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
+    <hyperlink ref="B169" r:id="rId153" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
+    <hyperlink ref="B170" r:id="rId154" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
+    <hyperlink ref="B171" r:id="rId155" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
+    <hyperlink ref="B174" r:id="rId156" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
+    <hyperlink ref="B175" r:id="rId157" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
+    <hyperlink ref="B176" r:id="rId158" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
+    <hyperlink ref="B177" r:id="rId159" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
+    <hyperlink ref="B178" r:id="rId160" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
+    <hyperlink ref="B179" r:id="rId161" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
+    <hyperlink ref="B180" r:id="rId162" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
+    <hyperlink ref="B181" r:id="rId163" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
+    <hyperlink ref="B182" r:id="rId164" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
+    <hyperlink ref="B183" r:id="rId165" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
+    <hyperlink ref="B184" r:id="rId166" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
+    <hyperlink ref="B185" r:id="rId167" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
+    <hyperlink ref="B186" r:id="rId168" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
+    <hyperlink ref="B187" r:id="rId169" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
+    <hyperlink ref="B188" r:id="rId170" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
+    <hyperlink ref="B189" r:id="rId171" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
+    <hyperlink ref="B190" r:id="rId172" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
+    <hyperlink ref="B191" r:id="rId173" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
+    <hyperlink ref="B192" r:id="rId174" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
+    <hyperlink ref="B193" r:id="rId175" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
+    <hyperlink ref="B194" r:id="rId176" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
+    <hyperlink ref="B195" r:id="rId177" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
+    <hyperlink ref="B196" r:id="rId178" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
+    <hyperlink ref="B197" r:id="rId179" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
+    <hyperlink ref="B198" r:id="rId180" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
+    <hyperlink ref="B199" r:id="rId181" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
+    <hyperlink ref="B200" r:id="rId182" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
+    <hyperlink ref="B201" r:id="rId183" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
+    <hyperlink ref="B202" r:id="rId184" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
+    <hyperlink ref="B203" r:id="rId185" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
+    <hyperlink ref="B204" r:id="rId186" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
+    <hyperlink ref="B205" r:id="rId187" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
+    <hyperlink ref="B206" r:id="rId188" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
+    <hyperlink ref="B207" r:id="rId189" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
+    <hyperlink ref="B208" r:id="rId190" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
+    <hyperlink ref="B211" r:id="rId191" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
+    <hyperlink ref="B212" r:id="rId192" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
+    <hyperlink ref="B213" r:id="rId193" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
+    <hyperlink ref="B214" r:id="rId194" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
+    <hyperlink ref="B215" r:id="rId195" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
+    <hyperlink ref="B216" r:id="rId196" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
+    <hyperlink ref="B217" r:id="rId197" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
+    <hyperlink ref="B218" r:id="rId198" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
+    <hyperlink ref="B219" r:id="rId199" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
+    <hyperlink ref="B220" r:id="rId200" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
+    <hyperlink ref="B221" r:id="rId201" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
+    <hyperlink ref="B222" r:id="rId202" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
+    <hyperlink ref="B223" r:id="rId203" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
+    <hyperlink ref="B224" r:id="rId204" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
+    <hyperlink ref="B225" r:id="rId205" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
+    <hyperlink ref="B226" r:id="rId206" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
+    <hyperlink ref="B227" r:id="rId207" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
+    <hyperlink ref="B228" r:id="rId208" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
+    <hyperlink ref="B229" r:id="rId209" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
+    <hyperlink ref="B230" r:id="rId210" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
+    <hyperlink ref="B231" r:id="rId211" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
+    <hyperlink ref="B232" r:id="rId212" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
+    <hyperlink ref="B235" r:id="rId213" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
+    <hyperlink ref="B236" r:id="rId214" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
+    <hyperlink ref="B237" r:id="rId215" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
+    <hyperlink ref="B238" r:id="rId216" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
+    <hyperlink ref="B239" r:id="rId217" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
+    <hyperlink ref="B240" r:id="rId218" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
+    <hyperlink ref="B241" r:id="rId219" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
+    <hyperlink ref="B242" r:id="rId220" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
+    <hyperlink ref="B243" r:id="rId221" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
+    <hyperlink ref="B244" r:id="rId222" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
+    <hyperlink ref="B245" r:id="rId223" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
+    <hyperlink ref="B246" r:id="rId224" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
+    <hyperlink ref="B247" r:id="rId225" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
+    <hyperlink ref="B248" r:id="rId226" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
+    <hyperlink ref="B249" r:id="rId227" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
+    <hyperlink ref="B250" r:id="rId228" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
+    <hyperlink ref="B251" r:id="rId229" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
+    <hyperlink ref="B252" r:id="rId230" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
+    <hyperlink ref="B253" r:id="rId231" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
+    <hyperlink ref="B254" r:id="rId232" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
+    <hyperlink ref="B255" r:id="rId233" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
+    <hyperlink ref="B256" r:id="rId234" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
+    <hyperlink ref="B257" r:id="rId235" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
+    <hyperlink ref="B258" r:id="rId236" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
+    <hyperlink ref="B259" r:id="rId237" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
+    <hyperlink ref="B260" r:id="rId238" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
+    <hyperlink ref="B261" r:id="rId239" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
+    <hyperlink ref="B262" r:id="rId240" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
+    <hyperlink ref="B263" r:id="rId241" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
+    <hyperlink ref="B264" r:id="rId242" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
+    <hyperlink ref="B265" r:id="rId243" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
+    <hyperlink ref="B266" r:id="rId244" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
+    <hyperlink ref="B267" r:id="rId245" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
+    <hyperlink ref="B268" r:id="rId246" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
+    <hyperlink ref="B269" r:id="rId247" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
+    <hyperlink ref="B272" r:id="rId248" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
+    <hyperlink ref="B273" r:id="rId249" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
+    <hyperlink ref="B274" r:id="rId250" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
+    <hyperlink ref="B275" r:id="rId251" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
+    <hyperlink ref="B276" r:id="rId252" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
+    <hyperlink ref="B277" r:id="rId253" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
+    <hyperlink ref="B278" r:id="rId254" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
+    <hyperlink ref="B279" r:id="rId255" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
+    <hyperlink ref="B280" r:id="rId256" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
+    <hyperlink ref="B281" r:id="rId257" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
+    <hyperlink ref="B282" r:id="rId258" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
+    <hyperlink ref="B283" r:id="rId259" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
+    <hyperlink ref="B284" r:id="rId260" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
+    <hyperlink ref="B285" r:id="rId261" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
+    <hyperlink ref="B286" r:id="rId262" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
+    <hyperlink ref="B287" r:id="rId263" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
+    <hyperlink ref="B288" r:id="rId264" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
+    <hyperlink ref="B289" r:id="rId265" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
+    <hyperlink ref="B290" r:id="rId266" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
+    <hyperlink ref="B293" r:id="rId267" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
+    <hyperlink ref="B294" r:id="rId268" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
+    <hyperlink ref="B295" r:id="rId269" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
+    <hyperlink ref="B296" r:id="rId270" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
+    <hyperlink ref="B297" r:id="rId271" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
+    <hyperlink ref="B298" r:id="rId272" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
+    <hyperlink ref="B299" r:id="rId273" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
+    <hyperlink ref="B300" r:id="rId274" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
+    <hyperlink ref="B301" r:id="rId275" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
+    <hyperlink ref="B302" r:id="rId276" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
+    <hyperlink ref="B303" r:id="rId277" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
+    <hyperlink ref="B304" r:id="rId278" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
+    <hyperlink ref="B305" r:id="rId279" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
+    <hyperlink ref="B306" r:id="rId280" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
+    <hyperlink ref="B307" r:id="rId281" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
+    <hyperlink ref="B308" r:id="rId282" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
+    <hyperlink ref="B309" r:id="rId283" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
+    <hyperlink ref="B310" r:id="rId284" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
+    <hyperlink ref="B311" r:id="rId285" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
+    <hyperlink ref="B312" r:id="rId286" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
+    <hyperlink ref="B313" r:id="rId287" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
+    <hyperlink ref="B314" r:id="rId288" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
+    <hyperlink ref="B315" r:id="rId289" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
+    <hyperlink ref="B316" r:id="rId290" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
+    <hyperlink ref="B317" r:id="rId291" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
+    <hyperlink ref="B318" r:id="rId292" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
+    <hyperlink ref="B319" r:id="rId293" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
+    <hyperlink ref="B320" r:id="rId294" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
+    <hyperlink ref="B321" r:id="rId295" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
+    <hyperlink ref="B322" r:id="rId296" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
+    <hyperlink ref="B323" r:id="rId297" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
+    <hyperlink ref="B324" r:id="rId298" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
+    <hyperlink ref="B325" r:id="rId299" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
+    <hyperlink ref="B326" r:id="rId300" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
+    <hyperlink ref="B327" r:id="rId301" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
+    <hyperlink ref="B328" r:id="rId302" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
+    <hyperlink ref="B329" r:id="rId303" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
+    <hyperlink ref="B330" r:id="rId304" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
+    <hyperlink ref="B333" r:id="rId305" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
+    <hyperlink ref="B334" r:id="rId306" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
+    <hyperlink ref="B335" r:id="rId307" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
+    <hyperlink ref="B336" r:id="rId308" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
+    <hyperlink ref="B337" r:id="rId309" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
+    <hyperlink ref="B338" r:id="rId310" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
+    <hyperlink ref="B339" r:id="rId311" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
+    <hyperlink ref="B340" r:id="rId312" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
+    <hyperlink ref="B341" r:id="rId313" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
+    <hyperlink ref="B342" r:id="rId314" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
+    <hyperlink ref="B343" r:id="rId315" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
+    <hyperlink ref="B344" r:id="rId316" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
+    <hyperlink ref="B345" r:id="rId317" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
+    <hyperlink ref="B346" r:id="rId318" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
+    <hyperlink ref="B347" r:id="rId319" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
+    <hyperlink ref="B348" r:id="rId320" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
+    <hyperlink ref="B349" r:id="rId321" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
+    <hyperlink ref="B350" r:id="rId322" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
+    <hyperlink ref="B354" r:id="rId323" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
+    <hyperlink ref="B355" r:id="rId324" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
+    <hyperlink ref="B356" r:id="rId325" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
+    <hyperlink ref="B357" r:id="rId326" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
+    <hyperlink ref="B358" r:id="rId327" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
+    <hyperlink ref="B359" r:id="rId328" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
+    <hyperlink ref="B360" r:id="rId329" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
+    <hyperlink ref="B361" r:id="rId330" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
+    <hyperlink ref="B362" r:id="rId331" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
+    <hyperlink ref="B363" r:id="rId332" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
+    <hyperlink ref="B364" r:id="rId333" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
+    <hyperlink ref="B365" r:id="rId334" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
+    <hyperlink ref="B366" r:id="rId335" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
+    <hyperlink ref="B367" r:id="rId336" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
+    <hyperlink ref="B368" r:id="rId337" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
+    <hyperlink ref="B369" r:id="rId338" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
+    <hyperlink ref="B370" r:id="rId339" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
+    <hyperlink ref="B371" r:id="rId340" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
+    <hyperlink ref="B372" r:id="rId341" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
+    <hyperlink ref="B373" r:id="rId342" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
+    <hyperlink ref="B374" r:id="rId343" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
+    <hyperlink ref="B375" r:id="rId344" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
+    <hyperlink ref="B376" r:id="rId345" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
+    <hyperlink ref="B377" r:id="rId346" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
+    <hyperlink ref="B378" r:id="rId347" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
+    <hyperlink ref="B379" r:id="rId348" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
+    <hyperlink ref="B380" r:id="rId349" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
+    <hyperlink ref="B381" r:id="rId350" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
+    <hyperlink ref="B382" r:id="rId351" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
+    <hyperlink ref="B383" r:id="rId352" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
+    <hyperlink ref="B384" r:id="rId353" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
+    <hyperlink ref="B385" r:id="rId354" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
+    <hyperlink ref="B386" r:id="rId355" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
+    <hyperlink ref="B387" r:id="rId356" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
+    <hyperlink ref="B388" r:id="rId357" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
+    <hyperlink ref="B389" r:id="rId358" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
+    <hyperlink ref="B390" r:id="rId359" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
+    <hyperlink ref="B391" r:id="rId360" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
+    <hyperlink ref="B393" r:id="rId361" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
+    <hyperlink ref="B392" r:id="rId362" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
+    <hyperlink ref="B394" r:id="rId363" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
+    <hyperlink ref="B395" r:id="rId364" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
+    <hyperlink ref="B396" r:id="rId365" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
+    <hyperlink ref="B399" r:id="rId366" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
+    <hyperlink ref="B400" r:id="rId367" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
+    <hyperlink ref="B401" r:id="rId368" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
+    <hyperlink ref="B402" r:id="rId369" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
+    <hyperlink ref="B403" r:id="rId370" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
+    <hyperlink ref="B404" r:id="rId371" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
+    <hyperlink ref="B407" r:id="rId372" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
+    <hyperlink ref="B408" r:id="rId373" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
+    <hyperlink ref="B409" r:id="rId374" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
+    <hyperlink ref="B410" r:id="rId375" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
+    <hyperlink ref="B411" r:id="rId376" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
+    <hyperlink ref="B412" r:id="rId377" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
+    <hyperlink ref="B413" r:id="rId378" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
+    <hyperlink ref="B414" r:id="rId379" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
+    <hyperlink ref="B415" r:id="rId380" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
+    <hyperlink ref="B416" r:id="rId381" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
+    <hyperlink ref="B417" r:id="rId382" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
+    <hyperlink ref="B418" r:id="rId383" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
+    <hyperlink ref="B419" r:id="rId384" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
+    <hyperlink ref="B420" r:id="rId385" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
+    <hyperlink ref="B421" r:id="rId386" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
+    <hyperlink ref="B422" r:id="rId387" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
+    <hyperlink ref="B423" r:id="rId388" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
+    <hyperlink ref="B424" r:id="rId389" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
+    <hyperlink ref="B425" r:id="rId390" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
+    <hyperlink ref="B426" r:id="rId391" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
+    <hyperlink ref="B427" r:id="rId392" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
+    <hyperlink ref="B428" r:id="rId393" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
+    <hyperlink ref="B429" r:id="rId394" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
+    <hyperlink ref="B430" r:id="rId395" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
+    <hyperlink ref="B431" r:id="rId396" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
+    <hyperlink ref="B432" r:id="rId397" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
+    <hyperlink ref="B433" r:id="rId398" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
+    <hyperlink ref="B434" r:id="rId399" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
+    <hyperlink ref="B435" r:id="rId400" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
+    <hyperlink ref="B436" r:id="rId401" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
+    <hyperlink ref="B437" r:id="rId402" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
+    <hyperlink ref="B438" r:id="rId403" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
+    <hyperlink ref="B439" r:id="rId404" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
+    <hyperlink ref="B440" r:id="rId405" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
+    <hyperlink ref="B441" r:id="rId406" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
+    <hyperlink ref="B442" r:id="rId407" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
+    <hyperlink ref="B443" r:id="rId408" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
+    <hyperlink ref="B444" r:id="rId409" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
+    <hyperlink ref="B445" r:id="rId410" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
+    <hyperlink ref="B446" r:id="rId411" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
+    <hyperlink ref="B448" r:id="rId412" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
+    <hyperlink ref="B447" r:id="rId413" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
+    <hyperlink ref="B449" r:id="rId414" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
+    <hyperlink ref="B450" r:id="rId415" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
+    <hyperlink ref="B451" r:id="rId416" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
+    <hyperlink ref="B452" r:id="rId417" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
+    <hyperlink ref="B453" r:id="rId418" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
+    <hyperlink ref="B454" r:id="rId419" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
+    <hyperlink ref="B455" r:id="rId420" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
+    <hyperlink ref="B456" r:id="rId421" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
+    <hyperlink ref="B457" r:id="rId422" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
+    <hyperlink ref="B458" r:id="rId423" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
+    <hyperlink ref="B459" r:id="rId424" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
+    <hyperlink ref="B466" r:id="rId425" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
+    <hyperlink ref="B465" r:id="rId426" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
+    <hyperlink ref="B464" r:id="rId427" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
+    <hyperlink ref="B463" r:id="rId428" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
+    <hyperlink ref="B462" r:id="rId429" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
+    <hyperlink ref="B461" r:id="rId430" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
+    <hyperlink ref="B460" r:id="rId431" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
+    <hyperlink ref="B469" r:id="rId432" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
+    <hyperlink ref="B470" r:id="rId433" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
+    <hyperlink ref="B471" r:id="rId434" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
+    <hyperlink ref="B472" r:id="rId435" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
+    <hyperlink ref="B473" r:id="rId436" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
+    <hyperlink ref="B474" r:id="rId437" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
+    <hyperlink ref="B475" r:id="rId438" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
+    <hyperlink ref="B478" r:id="rId439" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
+    <hyperlink ref="B476" r:id="rId440" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
+    <hyperlink ref="B477" r:id="rId441" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
+    <hyperlink ref="B353" r:id="rId442" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
+    <hyperlink ref="B12" r:id="rId443" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
+    <hyperlink ref="B31" r:id="rId444" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
+    <hyperlink ref="B36" r:id="rId445" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId446"/>

</xml_diff>